<commit_message>
Actualizar resultados de simulaciones y archivos Excel
- Actualización de todos los resultados de simulaciones (Día, Noche, Promedio)
- Actualización de resultados Monte Carlo para cada turno
- Eliminación de archivos obsoletos (results_caso_4.xlsx, results_montecarlo.xlsx)
- Actualización de top10_simulaciones.xlsx y respaldo de presentación
</commit_message>
<xml_diff>
--- a/Sims caso base/top10_simulaciones.xlsx
+++ b/Sims caso base/top10_simulaciones.xlsx
@@ -562,76 +562,76 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>7391</v>
+        <v>8873</v>
       </c>
       <c r="B2" t="n">
-        <v>93.56738643470854</v>
+        <v>93.2919385166476</v>
       </c>
       <c r="C2" t="n">
-        <v>9.367603049605739</v>
+        <v>9.41266559868745</v>
       </c>
       <c r="D2" t="n">
-        <v>9.988402149325337</v>
+        <v>9.911319757248862</v>
       </c>
       <c r="E2" t="n">
-        <v>25.13781168920708</v>
+        <v>24.94381843306821</v>
       </c>
       <c r="F2" t="n">
-        <v>0.02007391993459141</v>
+        <v>0.02056114049330139</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2177819808152502</v>
+        <v>0.1842869911555627</v>
       </c>
       <c r="H2" t="n">
         <v>23.84</v>
       </c>
       <c r="I2" t="n">
-        <v>0.4785622512406593</v>
+        <v>0.4901775893603053</v>
       </c>
       <c r="J2" t="n">
-        <v>23.36143774875934</v>
+        <v>23.3498224106397</v>
       </c>
       <c r="K2" t="n">
-        <v>7.734036474916924</v>
+        <v>7.730191101629033</v>
       </c>
       <c r="L2" t="n">
-        <v>31.09547422367626</v>
+        <v>31.08001351226873</v>
       </c>
       <c r="M2" t="n">
-        <v>9.488710790702273</v>
+        <v>9.483992990995816</v>
       </c>
       <c r="N2" t="n">
-        <v>21.60676343297399</v>
+        <v>21.59602052127291</v>
       </c>
       <c r="O2" t="n">
-        <v>1.754674315785349</v>
+        <v>1.753801889366783</v>
       </c>
       <c r="P2" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q2" t="n">
-        <v>27.30368123932124</v>
+        <v>22.55687474108279</v>
       </c>
       <c r="R2" t="n">
-        <v>2.008935295150894</v>
+        <v>2.096001102501442</v>
       </c>
       <c r="S2" t="n">
-        <v>3.285568536361338</v>
+        <v>3.4279627079976</v>
       </c>
       <c r="T2" t="n">
-        <v>2.326458288419646</v>
+        <v>2.427285313380355</v>
       </c>
       <c r="U2" t="n">
-        <v>7.217300382520526</v>
+        <v>7.530092977788444</v>
       </c>
       <c r="V2" t="n">
-        <v>0.1786222046916584</v>
+        <v>0.1863635622653705</v>
       </c>
       <c r="W2" t="n">
-        <v>24.54710183583333</v>
+        <v>25.61095553217273</v>
       </c>
       <c r="X2" t="n">
-        <v>10.84900116792675</v>
+        <v>8.962877872246509</v>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
@@ -641,76 +641,76 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2146</v>
+        <v>8204</v>
       </c>
       <c r="B3" t="n">
-        <v>92.924440056622</v>
+        <v>93.58560605668971</v>
       </c>
       <c r="C3" t="n">
-        <v>9.401960638903748</v>
+        <v>9.446733462800987</v>
       </c>
       <c r="D3" t="n">
-        <v>9.883517239172022</v>
+        <v>9.906663125958598</v>
       </c>
       <c r="E3" t="n">
-        <v>24.87384783582423</v>
+        <v>24.9320990891</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0204453974518386</v>
+        <v>0.02092948547434884</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1395984808732512</v>
+        <v>0.2199975214305451</v>
       </c>
       <c r="H3" t="n">
         <v>23.84</v>
       </c>
       <c r="I3" t="n">
-        <v>0.4874182752518322</v>
+        <v>0.4989589337084762</v>
       </c>
       <c r="J3" t="n">
-        <v>23.35258172474817</v>
+        <v>23.34104106629152</v>
       </c>
       <c r="K3" t="n">
-        <v>7.731104600027128</v>
+        <v>7.727283950184932</v>
       </c>
       <c r="L3" t="n">
-        <v>31.08368632477529</v>
+        <v>31.06832501647646</v>
       </c>
       <c r="M3" t="n">
-        <v>9.485113741089949</v>
+        <v>9.480426274008211</v>
       </c>
       <c r="N3" t="n">
-        <v>21.59857258368535</v>
+        <v>21.58789874246824</v>
       </c>
       <c r="O3" t="n">
-        <v>1.754009141062821</v>
+        <v>1.753142323823279</v>
       </c>
       <c r="P3" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q3" t="n">
-        <v>17.18369611749061</v>
+        <v>26.45395955207919</v>
       </c>
       <c r="R3" t="n">
-        <v>2.210568453819117</v>
+        <v>2.004995767610073</v>
       </c>
       <c r="S3" t="n">
-        <v>3.615335036858661</v>
+        <v>3.279125527585749</v>
       </c>
       <c r="T3" t="n">
-        <v>2.559960648767536</v>
+        <v>2.321896097431253</v>
       </c>
       <c r="U3" t="n">
-        <v>7.941687612262379</v>
+        <v>7.203147236973257</v>
       </c>
       <c r="V3" t="n">
-        <v>0.1965501884486243</v>
+        <v>0.1782719260657198</v>
       </c>
       <c r="W3" t="n">
-        <v>27.01084951912437</v>
+        <v>24.4989649028206</v>
       </c>
       <c r="X3" t="n">
-        <v>6.827868286840152</v>
+        <v>10.51136788337076</v>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
@@ -720,76 +720,76 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8511</v>
+        <v>6956</v>
       </c>
       <c r="B4" t="n">
-        <v>93.09690970216154</v>
+        <v>93.74316609712963</v>
       </c>
       <c r="C4" t="n">
-        <v>9.435776942939352</v>
+        <v>9.521957006527122</v>
       </c>
       <c r="D4" t="n">
-        <v>9.866374572559659</v>
+        <v>9.844947423399461</v>
       </c>
       <c r="E4" t="n">
-        <v>24.8307048867609</v>
+        <v>24.77677918046943</v>
       </c>
       <c r="F4" t="n">
-        <v>0.02081102254144144</v>
+        <v>0.0217428095705054</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1605711171328535</v>
+        <v>0.2391571214103433</v>
       </c>
       <c r="H4" t="n">
         <v>23.84</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4961347773879639</v>
+        <v>0.5183485801608487</v>
       </c>
       <c r="J4" t="n">
-        <v>23.34386522261204</v>
+        <v>23.32165141983915</v>
       </c>
       <c r="K4" t="n">
-        <v>7.728218915242675</v>
+        <v>7.720864814748528</v>
       </c>
       <c r="L4" t="n">
-        <v>31.07208413785471</v>
+        <v>31.04251623458768</v>
       </c>
       <c r="M4" t="n">
-        <v>9.481573361051453</v>
+        <v>9.472550784943746</v>
       </c>
       <c r="N4" t="n">
-        <v>21.59051077680326</v>
+        <v>21.56996544964393</v>
       </c>
       <c r="O4" t="n">
-        <v>1.753354445808778</v>
+        <v>1.751685970195217</v>
       </c>
       <c r="P4" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q4" t="n">
-        <v>19.41804299541461</v>
+        <v>27.68210453675147</v>
       </c>
       <c r="R4" t="n">
-        <v>2.157490247689351</v>
+        <v>1.957372040072518</v>
       </c>
       <c r="S4" t="n">
-        <v>3.528526823350042</v>
+        <v>3.201237991257762</v>
       </c>
       <c r="T4" t="n">
-        <v>2.498493147607542</v>
+        <v>2.266745184446342</v>
       </c>
       <c r="U4" t="n">
-        <v>7.75099886368569</v>
+        <v>7.032054246669635</v>
       </c>
       <c r="V4" t="n">
-        <v>0.1918307999133829</v>
+        <v>0.174037516311993</v>
       </c>
       <c r="W4" t="n">
-        <v>26.36228899341921</v>
+        <v>23.91705243780089</v>
       </c>
       <c r="X4" t="n">
-        <v>7.715676479284223</v>
+        <v>10.99936604948999</v>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
@@ -799,76 +799,76 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6633</v>
+        <v>4768</v>
       </c>
       <c r="B5" t="n">
-        <v>93.45225714002011</v>
+        <v>93.47642992732501</v>
       </c>
       <c r="C5" t="n">
-        <v>9.503756404348627</v>
+        <v>9.619543453054073</v>
       </c>
       <c r="D5" t="n">
-        <v>9.833191547003375</v>
+        <v>9.71734577462172</v>
       </c>
       <c r="E5" t="n">
-        <v>24.74719316634339</v>
+        <v>24.45564411099048</v>
       </c>
       <c r="F5" t="n">
-        <v>0.02154602293186707</v>
+        <v>0.02279792349477916</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2037820400559861</v>
+        <v>0.206721496874255</v>
       </c>
       <c r="H5" t="n">
         <v>23.84</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5136571866957109</v>
+        <v>0.5435024961155351</v>
       </c>
       <c r="J5" t="n">
-        <v>23.32634281330429</v>
+        <v>23.29649750388446</v>
       </c>
       <c r="K5" t="n">
-        <v>7.722417947246957</v>
+        <v>7.712537360523632</v>
       </c>
       <c r="L5" t="n">
-        <v>31.04876076055125</v>
+        <v>31.0090348644081</v>
       </c>
       <c r="M5" t="n">
-        <v>9.474456287347959</v>
+        <v>9.462334023616188</v>
       </c>
       <c r="N5" t="n">
-        <v>21.57430447320329</v>
+        <v>21.54670084079191</v>
       </c>
       <c r="O5" t="n">
-        <v>1.752038340101002</v>
+        <v>1.749796663092556</v>
       </c>
       <c r="P5" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q5" t="n">
-        <v>23.80292000201907</v>
+        <v>22.8203235835307</v>
       </c>
       <c r="R5" t="n">
-        <v>2.047967289984827</v>
+        <v>2.043020636997077</v>
       </c>
       <c r="S5" t="n">
-        <v>3.349404486900579</v>
+        <v>3.341314347085686</v>
       </c>
       <c r="T5" t="n">
-        <v>2.371659499286984</v>
+        <v>2.365931001275594</v>
       </c>
       <c r="U5" t="n">
-        <v>7.357526716303128</v>
+        <v>7.339755372155386</v>
       </c>
       <c r="V5" t="n">
-        <v>0.1820926902705514</v>
+        <v>0.1816528642270502</v>
       </c>
       <c r="W5" t="n">
-        <v>25.0240322548254</v>
+        <v>24.96358929534837</v>
       </c>
       <c r="X5" t="n">
-        <v>9.457988636714376</v>
+        <v>9.067558145003655</v>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
@@ -878,76 +878,76 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1642</v>
+        <v>4749</v>
       </c>
       <c r="B6" t="n">
-        <v>93.31122897260188</v>
+        <v>92.90876245601163</v>
       </c>
       <c r="C6" t="n">
-        <v>9.544681597943525</v>
+        <v>9.56464001418291</v>
       </c>
       <c r="D6" t="n">
-        <v>9.776253719422815</v>
+        <v>9.713775146606881</v>
       </c>
       <c r="E6" t="n">
-        <v>24.6038977356714</v>
+        <v>24.44665791146554</v>
       </c>
       <c r="F6" t="n">
-        <v>0.02198851001027146</v>
+        <v>0.0222043023014152</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1866327472145239</v>
+        <v>0.1376920548816143</v>
       </c>
       <c r="H6" t="n">
         <v>23.84</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5242060786448716</v>
+        <v>0.5293505668657384</v>
       </c>
       <c r="J6" t="n">
-        <v>23.31579392135513</v>
+        <v>23.31064943313426</v>
       </c>
       <c r="K6" t="n">
-        <v>7.718925631577767</v>
+        <v>7.717222497550962</v>
       </c>
       <c r="L6" t="n">
-        <v>31.03471955293289</v>
+        <v>31.02787193068522</v>
       </c>
       <c r="M6" t="n">
-        <v>9.470171645882631</v>
+        <v>9.46808211006643</v>
       </c>
       <c r="N6" t="n">
-        <v>21.56454790705026</v>
+        <v>21.55978982061879</v>
       </c>
       <c r="O6" t="n">
-        <v>1.751246014304865</v>
+        <v>1.750859612515467</v>
       </c>
       <c r="P6" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q6" t="n">
-        <v>21.3610942576547</v>
+        <v>15.60641671224556</v>
       </c>
       <c r="R6" t="n">
-        <v>2.093023840759485</v>
+        <v>2.219451783831041</v>
       </c>
       <c r="S6" t="n">
-        <v>3.423093463314856</v>
+        <v>3.629863523493222</v>
       </c>
       <c r="T6" t="n">
-        <v>2.423837479459029</v>
+        <v>2.570248036711237</v>
       </c>
       <c r="U6" t="n">
-        <v>7.519396868082491</v>
+        <v>7.973601861192088</v>
       </c>
       <c r="V6" t="n">
-        <v>0.1860988424122343</v>
+        <v>0.1973400396676077</v>
       </c>
       <c r="W6" t="n">
-        <v>25.5745764873383</v>
+        <v>27.11939458126271</v>
       </c>
       <c r="X6" t="n">
-        <v>8.487739602517063</v>
+        <v>6.201143049328707</v>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
@@ -957,76 +957,76 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>126</v>
+        <v>8651</v>
       </c>
       <c r="B7" t="n">
-        <v>93.7244984845436</v>
+        <v>93.18402359693002</v>
       </c>
       <c r="C7" t="n">
-        <v>9.637947620174469</v>
+        <v>9.619080689754348</v>
       </c>
       <c r="D7" t="n">
-        <v>9.724528725219091</v>
+        <v>9.687414691944927</v>
       </c>
       <c r="E7" t="n">
-        <v>24.47372144275889</v>
+        <v>24.3803165552178</v>
       </c>
       <c r="F7" t="n">
-        <v>0.02299691109689485</v>
+        <v>0.02279292005404983</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2368871042871666</v>
+        <v>0.171164332086249</v>
       </c>
       <c r="H7" t="n">
         <v>23.84</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5482463605499732</v>
+        <v>0.543383214088548</v>
       </c>
       <c r="J7" t="n">
-        <v>23.29175363945003</v>
+        <v>23.29661678591145</v>
       </c>
       <c r="K7" t="n">
-        <v>7.710966856988596</v>
+        <v>7.712576850025839</v>
       </c>
       <c r="L7" t="n">
-        <v>31.00272049643862</v>
+        <v>31.00919363593729</v>
       </c>
       <c r="M7" t="n">
-        <v>9.460407209088215</v>
+        <v>9.462382472374728</v>
       </c>
       <c r="N7" t="n">
-        <v>21.54231328735041</v>
+        <v>21.54681116356256</v>
       </c>
       <c r="O7" t="n">
-        <v>1.74944035209962</v>
+        <v>1.749805622348888</v>
       </c>
       <c r="P7" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q7" t="n">
-        <v>25.92408053619037</v>
+        <v>18.89925790727828</v>
       </c>
       <c r="R7" t="n">
-        <v>1.96573198841847</v>
+        <v>2.134584130882383</v>
       </c>
       <c r="S7" t="n">
-        <v>3.214910498937511</v>
+        <v>3.49106438399082</v>
       </c>
       <c r="T7" t="n">
-        <v>2.276426467445922</v>
+        <v>2.471966596239906</v>
       </c>
       <c r="U7" t="n">
-        <v>7.062088194771765</v>
+        <v>7.668706354816922</v>
       </c>
       <c r="V7" t="n">
-        <v>0.1747808316433861</v>
+        <v>0.1897941285009878</v>
       </c>
       <c r="W7" t="n">
-        <v>24.01920231982334</v>
+        <v>26.08240004762721</v>
       </c>
       <c r="X7" t="n">
-        <v>10.30082271871513</v>
+        <v>7.509539439455748</v>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
@@ -1036,76 +1036,76 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7243</v>
+        <v>7475</v>
       </c>
       <c r="B8" t="n">
-        <v>93.50639544479303</v>
+        <v>93.07507284982938</v>
       </c>
       <c r="C8" t="n">
-        <v>9.626207853317887</v>
+        <v>9.728485214313201</v>
       </c>
       <c r="D8" t="n">
-        <v>9.713731187776501</v>
+        <v>9.567272889811363</v>
       </c>
       <c r="E8" t="n">
-        <v>24.44654728027712</v>
+        <v>24.07795568178826</v>
       </c>
       <c r="F8" t="n">
-        <v>0.02286997962312008</v>
+        <v>0.0239758121599604</v>
       </c>
       <c r="G8" t="n">
-        <v>0.210365360675457</v>
+        <v>0.1579157144410664</v>
       </c>
       <c r="H8" t="n">
         <v>23.84</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5452203142151828</v>
+        <v>0.5715833618934559</v>
       </c>
       <c r="J8" t="n">
-        <v>23.29477968578482</v>
+        <v>23.26841663810654</v>
       </c>
       <c r="K8" t="n">
-        <v>7.711968659744905</v>
+        <v>7.703240910428853</v>
       </c>
       <c r="L8" t="n">
-        <v>31.00674834552972</v>
+        <v>30.9716575485354</v>
       </c>
       <c r="M8" t="n">
-        <v>9.461636297760705</v>
+        <v>9.450928423627664</v>
       </c>
       <c r="N8" t="n">
-        <v>21.54511204776902</v>
+        <v>21.52072912490774</v>
       </c>
       <c r="O8" t="n">
-        <v>1.749667638015801</v>
+        <v>1.747687513198811</v>
       </c>
       <c r="P8" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q8" t="n">
-        <v>23.14940861060962</v>
+        <v>16.57614248402955</v>
       </c>
       <c r="R8" t="n">
-        <v>2.033786144469888</v>
+        <v>2.171332993453944</v>
       </c>
       <c r="S8" t="n">
-        <v>3.326211542047698</v>
+        <v>3.551166323014754</v>
       </c>
       <c r="T8" t="n">
-        <v>2.355236947698514</v>
+        <v>2.51452381355097</v>
       </c>
       <c r="U8" t="n">
-        <v>7.306579536871023</v>
+        <v>7.800730308268842</v>
       </c>
       <c r="V8" t="n">
-        <v>0.1808317897910558</v>
+        <v>0.193061611962644</v>
       </c>
       <c r="W8" t="n">
-        <v>24.85075339216407</v>
+        <v>26.5314329627602</v>
       </c>
       <c r="X8" t="n">
-        <v>9.198318675491565</v>
+        <v>6.586459444522411</v>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
@@ -1115,76 +1115,76 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5133</v>
+        <v>7246</v>
       </c>
       <c r="B9" t="n">
-        <v>93.71206111065425</v>
+        <v>93.46372393839222</v>
       </c>
       <c r="C9" t="n">
-        <v>9.689085103528299</v>
+        <v>9.772116835343846</v>
       </c>
       <c r="D9" t="n">
-        <v>9.671920528030951</v>
+        <v>9.564327311391951</v>
       </c>
       <c r="E9" t="n">
-        <v>24.3413223928955</v>
+        <v>24.07054254458012</v>
       </c>
       <c r="F9" t="n">
-        <v>0.02354981442168233</v>
+        <v>0.02444756138873632</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2353746960150309</v>
+        <v>0.2051764245029873</v>
       </c>
       <c r="H9" t="n">
         <v>23.84</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5614275758129067</v>
+        <v>0.5828298635074739</v>
       </c>
       <c r="J9" t="n">
-        <v>23.27857242418709</v>
+        <v>23.25717013649253</v>
       </c>
       <c r="K9" t="n">
-        <v>7.706603084487792</v>
+        <v>7.699517644137048</v>
       </c>
       <c r="L9" t="n">
-        <v>30.98517550867489</v>
+        <v>30.95668778062957</v>
       </c>
       <c r="M9" t="n">
-        <v>9.455053397356032</v>
+        <v>9.446360434175547</v>
       </c>
       <c r="N9" t="n">
-        <v>21.53012211131885</v>
+        <v>21.51032734645403</v>
       </c>
       <c r="O9" t="n">
-        <v>1.74845031286824</v>
+        <v>1.746842790038499</v>
       </c>
       <c r="P9" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q9" t="n">
-        <v>25.15380745062837</v>
+        <v>21.12143208625189</v>
       </c>
       <c r="R9" t="n">
-        <v>1.970743137704722</v>
+        <v>2.050461270232569</v>
       </c>
       <c r="S9" t="n">
-        <v>3.223106120999438</v>
+        <v>3.353483335558407</v>
       </c>
       <c r="T9" t="n">
-        <v>2.282229655741558</v>
+        <v>2.374547666483071</v>
       </c>
       <c r="U9" t="n">
-        <v>7.08009124830357</v>
+        <v>7.366486589047402</v>
       </c>
       <c r="V9" t="n">
-        <v>0.1752263923021639</v>
+        <v>0.1823144396974168</v>
       </c>
       <c r="W9" t="n">
-        <v>24.08043335705044</v>
+        <v>25.05450610197502</v>
       </c>
       <c r="X9" t="n">
-        <v>9.994757996832506</v>
+        <v>8.392510861942977</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
@@ -1194,76 +1194,76 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>5577</v>
+        <v>6560</v>
       </c>
       <c r="B10" t="n">
-        <v>93.52787729548201</v>
+        <v>93.90574988040341</v>
       </c>
       <c r="C10" t="n">
-        <v>9.758709887431371</v>
+        <v>9.822330354842688</v>
       </c>
       <c r="D10" t="n">
-        <v>9.584041166746875</v>
+        <v>9.560434895585161</v>
       </c>
       <c r="E10" t="n">
-        <v>24.12015640435186</v>
+        <v>24.06074650171917</v>
       </c>
       <c r="F10" t="n">
-        <v>0.02430260419511046</v>
+        <v>0.02499047472860661</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2129775944936057</v>
+        <v>0.2589276180542164</v>
       </c>
       <c r="H10" t="n">
         <v>23.84</v>
       </c>
       <c r="I10" t="n">
-        <v>0.5793740840114334</v>
+        <v>0.5957729175299816</v>
       </c>
       <c r="J10" t="n">
-        <v>23.26062591598857</v>
+        <v>23.24422708247002</v>
       </c>
       <c r="K10" t="n">
-        <v>7.700661714333372</v>
+        <v>7.695232717285224</v>
       </c>
       <c r="L10" t="n">
-        <v>30.96128763032194</v>
+        <v>30.93945979975524</v>
       </c>
       <c r="M10" t="n">
-        <v>9.447764067485577</v>
+        <v>9.441103356349739</v>
       </c>
       <c r="N10" t="n">
-        <v>21.51352356283636</v>
+        <v>21.4983564434055</v>
       </c>
       <c r="O10" t="n">
-        <v>1.747102353152205</v>
+        <v>1.745870639064515</v>
       </c>
       <c r="P10" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q10" t="n">
-        <v>22.05527884003055</v>
+        <v>26.07566056402723</v>
       </c>
       <c r="R10" t="n">
-        <v>2.030034410724228</v>
+        <v>1.912860146800941</v>
       </c>
       <c r="S10" t="n">
-        <v>3.320075665804546</v>
+        <v>3.128439789951842</v>
       </c>
       <c r="T10" t="n">
-        <v>2.350892232321368</v>
+        <v>2.215197947815641</v>
       </c>
       <c r="U10" t="n">
-        <v>7.29310105926001</v>
+        <v>6.872140831284336</v>
       </c>
       <c r="V10" t="n">
-        <v>0.1804982086375545</v>
+        <v>0.1700797917748413</v>
       </c>
       <c r="W10" t="n">
-        <v>24.80491110419296</v>
+        <v>23.37316335402577</v>
       </c>
       <c r="X10" t="n">
-        <v>8.763570882517007</v>
+        <v>10.36105239560823</v>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
@@ -1273,76 +1273,76 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9079</v>
+        <v>5402</v>
       </c>
       <c r="B11" t="n">
-        <v>93.77817884391402</v>
+        <v>94.13728388896972</v>
       </c>
       <c r="C11" t="n">
-        <v>9.83488341424</v>
+        <v>10.0338801679741</v>
       </c>
       <c r="D11" t="n">
-        <v>9.535260856080093</v>
+        <v>9.38194221109346</v>
       </c>
       <c r="E11" t="n">
-        <v>23.99739099649677</v>
+        <v>23.61153396265891</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02512619959854214</v>
+        <v>0.0272777713917843</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2434147378764777</v>
+        <v>0.2870825929670343</v>
       </c>
       <c r="H11" t="n">
         <v>23.84</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5990085984292447</v>
+        <v>0.6503020699801377</v>
       </c>
       <c r="J11" t="n">
-        <v>23.24099140157076</v>
+        <v>23.18969793001986</v>
       </c>
       <c r="K11" t="n">
-        <v>7.694161512919925</v>
+        <v>7.677180298657084</v>
       </c>
       <c r="L11" t="n">
-        <v>30.93515291449068</v>
+        <v>30.86687822867695</v>
       </c>
       <c r="M11" t="n">
-        <v>9.439789120445496</v>
+        <v>9.418955260721971</v>
       </c>
       <c r="N11" t="n">
-        <v>21.49536379404518</v>
+        <v>21.44792296795497</v>
       </c>
       <c r="O11" t="n">
-        <v>1.745627607525572</v>
+        <v>1.741774962064887</v>
       </c>
       <c r="P11" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q11" t="n">
-        <v>24.38099993638814</v>
+        <v>26.48679583617827</v>
       </c>
       <c r="R11" t="n">
-        <v>1.953173968160957</v>
+        <v>1.844513454624174</v>
       </c>
       <c r="S11" t="n">
-        <v>3.194372138973076</v>
+        <v>3.016660310581655</v>
       </c>
       <c r="T11" t="n">
-        <v>2.261883584763363</v>
+        <v>2.136048694534807</v>
       </c>
       <c r="U11" t="n">
-        <v>7.016972254687973</v>
+        <v>6.626598523982524</v>
       </c>
       <c r="V11" t="n">
-        <v>0.1736642495063836</v>
+        <v>0.1640028231091684</v>
       </c>
       <c r="W11" t="n">
-        <v>23.86575636122942</v>
+        <v>22.53803779420557</v>
       </c>
       <c r="X11" t="n">
-        <v>9.687686230535279</v>
+        <v>10.52441524066368</v>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
@@ -1352,76 +1352,76 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9194</v>
+        <v>9204</v>
       </c>
       <c r="B12" t="n">
-        <v>92.35418792054283</v>
+        <v>92.62204019411423</v>
       </c>
       <c r="C12" t="n">
-        <v>13.16480938682608</v>
+        <v>13.26504622402237</v>
       </c>
       <c r="D12" t="n">
-        <v>7.0152316837159</v>
+        <v>6.98241367801494</v>
       </c>
       <c r="E12" t="n">
-        <v>17.6552335784078</v>
+        <v>17.5726405034602</v>
       </c>
       <c r="F12" t="n">
-        <v>0.02046512700638586</v>
+        <v>0.02159583768829981</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2041804836204563</v>
+        <v>0.2320600684964027</v>
       </c>
       <c r="H12" t="n">
         <v>23.84</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4878886278322389</v>
+        <v>0.5148447704890674</v>
       </c>
       <c r="J12" t="n">
-        <v>23.35211137216776</v>
+        <v>23.32515522951093</v>
       </c>
       <c r="K12" t="n">
-        <v>4.118044469367088</v>
+        <v>4.113290869471374</v>
       </c>
       <c r="L12" t="n">
-        <v>27.47015584153485</v>
+        <v>27.43844609898231</v>
       </c>
       <c r="M12" t="n">
-        <v>6.768646399354187</v>
+        <v>6.760833118789241</v>
       </c>
       <c r="N12" t="n">
-        <v>20.70150944218067</v>
+        <v>20.67761298019307</v>
       </c>
       <c r="O12" t="n">
-        <v>2.6506019299871</v>
+        <v>2.647542249317866</v>
       </c>
       <c r="P12" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q12" t="n">
-        <v>25.10910501397129</v>
+        <v>27.04343229534968</v>
       </c>
       <c r="R12" t="n">
-        <v>2.044683688240117</v>
+        <v>1.97533340521439</v>
       </c>
       <c r="S12" t="n">
-        <v>0.4480835963895672</v>
+        <v>0.4328857814866917</v>
       </c>
       <c r="T12" t="n">
-        <v>1.805337751654823</v>
+        <v>1.7441054521288</v>
       </c>
       <c r="U12" t="n">
-        <v>6.649123415692987</v>
+        <v>6.423602669670806</v>
       </c>
       <c r="V12" t="n">
-        <v>0.2215946682962728</v>
+        <v>0.2140787610428797</v>
       </c>
       <c r="W12" t="n">
-        <v>16.28322103077011</v>
+        <v>15.73093707919893</v>
       </c>
       <c r="X12" t="n">
-        <v>9.976995674482971</v>
+        <v>10.74559236116727</v>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
@@ -1431,76 +1431,76 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9500</v>
+        <v>1904</v>
       </c>
       <c r="B13" t="n">
-        <v>92.14635835830937</v>
+        <v>92.4399999827716</v>
       </c>
       <c r="C13" t="n">
-        <v>13.25058371476164</v>
+        <v>13.24769343194224</v>
       </c>
       <c r="D13" t="n">
-        <v>6.954135783139496</v>
+        <v>6.977818475168248</v>
       </c>
       <c r="E13" t="n">
-        <v>17.50147352542717</v>
+        <v>17.56107575645593</v>
       </c>
       <c r="F13" t="n">
-        <v>0.02143269493394124</v>
+        <v>0.02140009141462577</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1825484032100108</v>
+        <v>0.2131122900986593</v>
       </c>
       <c r="H13" t="n">
         <v>23.84</v>
       </c>
       <c r="I13" t="n">
-        <v>0.5109554472251591</v>
+        <v>0.5101781793246785</v>
       </c>
       <c r="J13" t="n">
-        <v>23.32904455277484</v>
+        <v>23.32982182067532</v>
       </c>
       <c r="K13" t="n">
-        <v>4.11397673491203</v>
+        <v>4.114113802765458</v>
       </c>
       <c r="L13" t="n">
-        <v>27.44302128768687</v>
+        <v>27.44393562344078</v>
       </c>
       <c r="M13" t="n">
-        <v>6.761960445286045</v>
+        <v>6.762185737615809</v>
       </c>
       <c r="N13" t="n">
-        <v>20.68106084240083</v>
+        <v>20.68174988582497</v>
       </c>
       <c r="O13" t="n">
-        <v>2.647983710374015</v>
+        <v>2.648071934850351</v>
       </c>
       <c r="P13" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q13" t="n">
-        <v>21.43545493343856</v>
+        <v>25.06249576694507</v>
       </c>
       <c r="R13" t="n">
-        <v>2.102339228983833</v>
+        <v>2.023666957389599</v>
       </c>
       <c r="S13" t="n">
-        <v>0.4607185590475154</v>
+        <v>0.443477870624739</v>
       </c>
       <c r="T13" t="n">
-        <v>1.856244268342641</v>
+        <v>1.78678119063806</v>
       </c>
       <c r="U13" t="n">
-        <v>6.836613934744102</v>
+        <v>6.580778938733927</v>
       </c>
       <c r="V13" t="n">
-        <v>0.2278431459948173</v>
+        <v>0.2193169587765666</v>
       </c>
       <c r="W13" t="n">
-        <v>16.74237171455463</v>
+        <v>16.11585036324269</v>
       </c>
       <c r="X13" t="n">
-        <v>8.517286499558374</v>
+        <v>9.958475689174341</v>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
@@ -1510,76 +1510,76 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>8272</v>
+        <v>9984</v>
       </c>
       <c r="B14" t="n">
-        <v>92.65910041637324</v>
+        <v>92.00666619795459</v>
       </c>
       <c r="C14" t="n">
-        <v>13.35402920645193</v>
+        <v>13.26567174911016</v>
       </c>
       <c r="D14" t="n">
-        <v>6.938662405471263</v>
+        <v>6.935695978164564</v>
       </c>
       <c r="E14" t="n">
-        <v>17.46253167584953</v>
+        <v>17.45506606824676</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02259960049203464</v>
+        <v>0.0216028938556565</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2359175067709226</v>
+        <v>0.1680084503128856</v>
       </c>
       <c r="H14" t="n">
         <v>23.84</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5387744757301058</v>
+        <v>0.5150129895188509</v>
       </c>
       <c r="J14" t="n">
-        <v>23.30122552426989</v>
+        <v>23.32498701048115</v>
       </c>
       <c r="K14" t="n">
-        <v>4.109070968805822</v>
+        <v>4.113261204768504</v>
       </c>
       <c r="L14" t="n">
-        <v>27.41029649307571</v>
+        <v>27.43824821524965</v>
       </c>
       <c r="M14" t="n">
-        <v>6.753897055893856</v>
+        <v>6.760784360237514</v>
       </c>
       <c r="N14" t="n">
-        <v>20.65639943718186</v>
+        <v>20.67746385501214</v>
       </c>
       <c r="O14" t="n">
-        <v>2.644826087088034</v>
+        <v>2.64752315546901</v>
       </c>
       <c r="P14" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q14" t="n">
-        <v>26.27186217294619</v>
+        <v>19.5726956641842</v>
       </c>
       <c r="R14" t="n">
-        <v>1.967429532132034</v>
+        <v>2.140105607373547</v>
       </c>
       <c r="S14" t="n">
-        <v>0.4311536818487292</v>
+        <v>0.4689948977050795</v>
       </c>
       <c r="T14" t="n">
-        <v>1.737126788122268</v>
+        <v>1.889589801953718</v>
       </c>
       <c r="U14" t="n">
-        <v>6.397900000896746</v>
+        <v>6.959426725945613</v>
       </c>
       <c r="V14" t="n">
-        <v>0.2132221707819929</v>
+        <v>0.231936115552971</v>
       </c>
       <c r="W14" t="n">
-        <v>15.66799310740546</v>
+        <v>17.04313133345721</v>
       </c>
       <c r="X14" t="n">
-        <v>10.43901226723336</v>
+        <v>7.777127056933362</v>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
@@ -1589,76 +1589,76 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2852</v>
+        <v>5056</v>
       </c>
       <c r="B15" t="n">
-        <v>91.86380813417159</v>
+        <v>92.26633056818045</v>
       </c>
       <c r="C15" t="n">
-        <v>13.27245091991609</v>
+        <v>13.36092209466642</v>
       </c>
       <c r="D15" t="n">
-        <v>6.921389929295167</v>
+        <v>6.905685843719757</v>
       </c>
       <c r="E15" t="n">
-        <v>17.41906203505715</v>
+        <v>17.37953956288951</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02167936555068583</v>
+        <v>0.02267735496385727</v>
       </c>
       <c r="G15" t="n">
-        <v>0.153138972218315</v>
+        <v>0.1950357917367453</v>
       </c>
       <c r="H15" t="n">
         <v>23.84</v>
       </c>
       <c r="I15" t="n">
-        <v>0.5168360747283502</v>
+        <v>0.5406281423383572</v>
       </c>
       <c r="J15" t="n">
-        <v>23.32316392527165</v>
+        <v>23.29937185766164</v>
       </c>
       <c r="K15" t="n">
-        <v>4.112939711527722</v>
+        <v>4.108744082666814</v>
       </c>
       <c r="L15" t="n">
-        <v>27.43610363679937</v>
+        <v>27.40811594032846</v>
       </c>
       <c r="M15" t="n">
-        <v>6.760255936107366</v>
+        <v>6.753359767696932</v>
       </c>
       <c r="N15" t="n">
-        <v>20.67584770069201</v>
+        <v>20.65475617263153</v>
       </c>
       <c r="O15" t="n">
-        <v>2.647316224579645</v>
+        <v>2.644615685030119</v>
       </c>
       <c r="P15" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q15" t="n">
-        <v>17.77749678516958</v>
+        <v>21.64478960823115</v>
       </c>
       <c r="R15" t="n">
-        <v>2.178524170470808</v>
+        <v>2.072860414342711</v>
       </c>
       <c r="S15" t="n">
-        <v>0.4774141598235916</v>
+        <v>0.4542584041797154</v>
       </c>
       <c r="T15" t="n">
-        <v>1.923511177041086</v>
+        <v>1.830216175463659</v>
       </c>
       <c r="U15" t="n">
-        <v>7.084360361870071</v>
+        <v>6.740751539096064</v>
       </c>
       <c r="V15" t="n">
-        <v>0.2360997662902077</v>
+        <v>0.2246483495626174</v>
       </c>
       <c r="W15" t="n">
-        <v>17.34908474727629</v>
+        <v>16.50761165983944</v>
       </c>
       <c r="X15" t="n">
-        <v>7.063812446922388</v>
+        <v>8.600464738837029</v>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
@@ -1668,76 +1668,76 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6464</v>
+        <v>6192</v>
       </c>
       <c r="B16" t="n">
-        <v>91.83987865952926</v>
+        <v>92.26826509347487</v>
       </c>
       <c r="C16" t="n">
-        <v>13.28531005299335</v>
+        <v>13.39615377132213</v>
       </c>
       <c r="D16" t="n">
-        <v>6.912889371282426</v>
+        <v>6.887668406061338</v>
       </c>
       <c r="E16" t="n">
-        <v>17.39766868070648</v>
+        <v>17.33419507753457</v>
       </c>
       <c r="F16" t="n">
-        <v>0.02182442159532278</v>
+        <v>0.02307478204007608</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1506482566816046</v>
+        <v>0.1952371481091239</v>
       </c>
       <c r="H16" t="n">
         <v>23.84</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5202942108324951</v>
+        <v>0.5501028038354138</v>
       </c>
       <c r="J16" t="n">
-        <v>23.3197057891675</v>
+        <v>23.28989719616458</v>
       </c>
       <c r="K16" t="n">
-        <v>4.112329884089378</v>
+        <v>4.10707326683542</v>
       </c>
       <c r="L16" t="n">
-        <v>27.43203567325688</v>
+        <v>27.39697046300001</v>
       </c>
       <c r="M16" t="n">
-        <v>6.759253589890496</v>
+        <v>6.750613522083202</v>
       </c>
       <c r="N16" t="n">
-        <v>20.67278208336639</v>
+        <v>20.64635694091681</v>
       </c>
       <c r="O16" t="n">
-        <v>2.646923705801118</v>
+        <v>2.643540255247782</v>
       </c>
       <c r="P16" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q16" t="n">
-        <v>17.37211984907071</v>
+        <v>21.29395327734208</v>
       </c>
       <c r="R16" t="n">
-        <v>2.185255469059649</v>
+        <v>2.073184960444796</v>
       </c>
       <c r="S16" t="n">
-        <v>0.4788892948273124</v>
+        <v>0.4543295270558124</v>
       </c>
       <c r="T16" t="n">
-        <v>1.929454525408361</v>
+        <v>1.830502730950757</v>
       </c>
       <c r="U16" t="n">
-        <v>7.106249926169185</v>
+        <v>6.741806933189172</v>
       </c>
       <c r="V16" t="n">
-        <v>0.2368292776012121</v>
+        <v>0.224683522575564</v>
       </c>
       <c r="W16" t="n">
-        <v>17.40269070274833</v>
+        <v>16.51019624343314</v>
       </c>
       <c r="X16" t="n">
-        <v>6.902737652112173</v>
+        <v>8.461061420646908</v>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
@@ -1747,76 +1747,76 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8330</v>
+        <v>2951</v>
       </c>
       <c r="B17" t="n">
-        <v>91.76322356437628</v>
+        <v>92.61297295850235</v>
       </c>
       <c r="C17" t="n">
-        <v>13.31512791911407</v>
+        <v>13.46340700538203</v>
       </c>
       <c r="D17" t="n">
-        <v>6.891651670326708</v>
+        <v>6.878866019684325</v>
       </c>
       <c r="E17" t="n">
-        <v>17.34421975871123</v>
+        <v>17.31204211173954</v>
       </c>
       <c r="F17" t="n">
-        <v>0.02216077877375769</v>
+        <v>0.0238334247932974</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1426695593086216</v>
+        <v>0.2311162991512305</v>
       </c>
       <c r="H17" t="n">
         <v>23.84</v>
       </c>
       <c r="I17" t="n">
-        <v>0.5283129659663833</v>
+        <v>0.5681888470722101</v>
       </c>
       <c r="J17" t="n">
-        <v>23.31168703403362</v>
+        <v>23.27181115292779</v>
       </c>
       <c r="K17" t="n">
-        <v>4.110915811087411</v>
+        <v>4.103883870847322</v>
       </c>
       <c r="L17" t="n">
-        <v>27.42260284512103</v>
+        <v>27.37569502377511</v>
       </c>
       <c r="M17" t="n">
-        <v>6.756929341037822</v>
+        <v>6.745371253858188</v>
       </c>
       <c r="N17" t="n">
-        <v>20.66567350408321</v>
+        <v>20.63032376991693</v>
       </c>
       <c r="O17" t="n">
-        <v>2.646013529950411</v>
+        <v>2.641487383010867</v>
       </c>
       <c r="P17" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q17" t="n">
-        <v>16.20234034090872</v>
+        <v>24.40481781860732</v>
       </c>
       <c r="R17" t="n">
-        <v>2.206542213946212</v>
+        <v>1.982294476243825</v>
       </c>
       <c r="S17" t="n">
-        <v>0.4835541930015665</v>
+        <v>0.4344112701280556</v>
       </c>
       <c r="T17" t="n">
-        <v>1.948249493243525</v>
+        <v>1.750251676306979</v>
       </c>
       <c r="U17" t="n">
-        <v>7.175472463954947</v>
+        <v>6.446239432827043</v>
       </c>
       <c r="V17" t="n">
-        <v>0.2391362501659051</v>
+        <v>0.2148331741751534</v>
       </c>
       <c r="W17" t="n">
-        <v>17.57221167756076</v>
+        <v>15.78637287048298</v>
       </c>
       <c r="X17" t="n">
-        <v>6.437930758894076</v>
+        <v>9.6971501643451</v>
       </c>
       <c r="Y17" t="inlineStr">
         <is>
@@ -1826,76 +1826,76 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6300</v>
+        <v>8828</v>
       </c>
       <c r="B18" t="n">
-        <v>91.83864675329787</v>
+        <v>91.75382950303654</v>
       </c>
       <c r="C18" t="n">
-        <v>13.45038655887874</v>
+        <v>13.37716287610233</v>
       </c>
       <c r="D18" t="n">
-        <v>6.827955936528401</v>
+        <v>6.858990232297348</v>
       </c>
       <c r="E18" t="n">
-        <v>17.18391670546103</v>
+        <v>17.26202071762274</v>
       </c>
       <c r="F18" t="n">
-        <v>0.02368654907019638</v>
+        <v>0.02286055732304825</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1505200328891402</v>
+        <v>0.1416917720867376</v>
       </c>
       <c r="H18" t="n">
         <v>23.84</v>
       </c>
       <c r="I18" t="n">
-        <v>0.5646873298334818</v>
+        <v>0.5449956865814704</v>
       </c>
       <c r="J18" t="n">
-        <v>23.27531267016652</v>
+        <v>23.29500431341853</v>
       </c>
       <c r="K18" t="n">
-        <v>4.104501348362289</v>
+        <v>4.107973885011945</v>
       </c>
       <c r="L18" t="n">
-        <v>27.3798140185288</v>
+        <v>27.40297819843047</v>
       </c>
       <c r="M18" t="n">
-        <v>6.746386174165497</v>
+        <v>6.752093828093269</v>
       </c>
       <c r="N18" t="n">
-        <v>20.63342784436331</v>
+        <v>20.65088437033721</v>
       </c>
       <c r="O18" t="n">
-        <v>2.641884825803209</v>
+        <v>2.644119943081324</v>
       </c>
       <c r="P18" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q18" t="n">
-        <v>15.99277993807641</v>
+        <v>15.59873093956328</v>
       </c>
       <c r="R18" t="n">
-        <v>2.189753947558399</v>
+        <v>2.210640797869676</v>
       </c>
       <c r="S18" t="n">
-        <v>0.479875116955006</v>
+        <v>0.4844523799607979</v>
       </c>
       <c r="T18" t="n">
-        <v>1.933426422433564</v>
+        <v>1.951868306426177</v>
       </c>
       <c r="U18" t="n">
-        <v>7.120878564766475</v>
+        <v>7.188800682149981</v>
       </c>
       <c r="V18" t="n">
-        <v>0.2373168047705742</v>
+        <v>0.2395804383551239</v>
       </c>
       <c r="W18" t="n">
-        <v>17.43851517776059</v>
+        <v>17.60485151731826</v>
       </c>
       <c r="X18" t="n">
-        <v>6.354662827542579</v>
+        <v>6.198089140367653</v>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
@@ -1905,76 +1905,76 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3059</v>
+        <v>7871</v>
       </c>
       <c r="B19" t="n">
-        <v>92.06781434907654</v>
+        <v>92.76395658682776</v>
       </c>
       <c r="C19" t="n">
-        <v>13.4894592405267</v>
+        <v>13.53804241511571</v>
       </c>
       <c r="D19" t="n">
-        <v>6.825167169968908</v>
+        <v>6.852095283972036</v>
       </c>
       <c r="E19" t="n">
-        <v>17.17689821666075</v>
+        <v>17.24466820117242</v>
       </c>
       <c r="F19" t="n">
-        <v>0.02412730418324785</v>
+        <v>0.02467534137202621</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1743730969387324</v>
+        <v>0.246831532121445</v>
       </c>
       <c r="H19" t="n">
         <v>23.84</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5751949317286287</v>
+        <v>0.5882601383091048</v>
       </c>
       <c r="J19" t="n">
-        <v>23.26480506827137</v>
+        <v>23.25173986169089</v>
       </c>
       <c r="K19" t="n">
-        <v>4.102648377931437</v>
+        <v>4.10034438490732</v>
       </c>
       <c r="L19" t="n">
-        <v>27.36745344620281</v>
+        <v>27.35208424659821</v>
       </c>
       <c r="M19" t="n">
-        <v>6.743340529144373</v>
+        <v>6.7395535583618</v>
       </c>
       <c r="N19" t="n">
-        <v>20.62411291705844</v>
+        <v>20.61253068823641</v>
       </c>
       <c r="O19" t="n">
-        <v>2.640692151212936</v>
+        <v>2.639209173454481</v>
       </c>
       <c r="P19" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q19" t="n">
-        <v>18.18871970663047</v>
+        <v>25.17496749180864</v>
       </c>
       <c r="R19" t="n">
-        <v>2.129227752596604</v>
+        <v>1.943454485992829</v>
       </c>
       <c r="S19" t="n">
-        <v>0.466611062827592</v>
+        <v>0.4258996540695437</v>
       </c>
       <c r="T19" t="n">
-        <v>1.879985283661337</v>
+        <v>1.715958205352369</v>
       </c>
       <c r="U19" t="n">
-        <v>6.924052942056262</v>
+        <v>6.319935354534394</v>
       </c>
       <c r="V19" t="n">
-        <v>0.2307572170099173</v>
+        <v>0.210623850842747</v>
       </c>
       <c r="W19" t="n">
-        <v>16.9565035021245</v>
+        <v>15.47706334269275</v>
       </c>
       <c r="X19" t="n">
-        <v>7.227210119056886</v>
+        <v>10.00316584885311</v>
       </c>
       <c r="Y19" t="inlineStr">
         <is>
@@ -1984,76 +1984,76 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>355</v>
+        <v>7411</v>
       </c>
       <c r="B20" t="n">
-        <v>92.16392197208746</v>
+        <v>91.88984197792088</v>
       </c>
       <c r="C20" t="n">
-        <v>13.63260384392602</v>
+        <v>13.42572941619263</v>
       </c>
       <c r="D20" t="n">
-        <v>6.760551617815179</v>
+        <v>6.84430909706057</v>
       </c>
       <c r="E20" t="n">
-        <v>17.01428025655546</v>
+        <v>17.22507270457234</v>
       </c>
       <c r="F20" t="n">
-        <v>0.02574203123020156</v>
+        <v>0.0234084068681827</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1843765238174068</v>
+        <v>0.1558487224353944</v>
       </c>
       <c r="H20" t="n">
         <v>23.84</v>
       </c>
       <c r="I20" t="n">
-        <v>0.6136900245280053</v>
+        <v>0.5580564197374756</v>
       </c>
       <c r="J20" t="n">
-        <v>23.226309975472</v>
+        <v>23.28194358026252</v>
       </c>
       <c r="K20" t="n">
-        <v>4.09585993377434</v>
+        <v>4.105670680857006</v>
       </c>
       <c r="L20" t="n">
-        <v>27.32216990924633</v>
+        <v>27.38761426111953</v>
       </c>
       <c r="M20" t="n">
-        <v>6.732182665638297</v>
+        <v>6.748308153939853</v>
       </c>
       <c r="N20" t="n">
-        <v>20.58998724360804</v>
+        <v>20.63930610717968</v>
       </c>
       <c r="O20" t="n">
-        <v>2.636322731863957</v>
+        <v>2.642637473082846</v>
       </c>
       <c r="P20" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q20" t="n">
-        <v>18.02578799402826</v>
+        <v>16.75571011567979</v>
       </c>
       <c r="R20" t="n">
-        <v>2.1069158973374</v>
+        <v>2.175398124648906</v>
       </c>
       <c r="S20" t="n">
-        <v>0.461721516144079</v>
+        <v>0.4767291003875467</v>
       </c>
       <c r="T20" t="n">
-        <v>1.860285202499361</v>
+        <v>1.920751058902452</v>
       </c>
       <c r="U20" t="n">
-        <v>6.851496839562378</v>
+        <v>7.074194748189832</v>
       </c>
       <c r="V20" t="n">
-        <v>0.2283391470689901</v>
+        <v>0.2357609779040298</v>
       </c>
       <c r="W20" t="n">
-        <v>16.77881886910194</v>
+        <v>17.32418989661402</v>
       </c>
       <c r="X20" t="n">
-        <v>7.162469898688067</v>
+        <v>6.657809876298242</v>
       </c>
       <c r="Y20" t="inlineStr">
         <is>
@@ -2063,76 +2063,76 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8687</v>
+        <v>3241</v>
       </c>
       <c r="B21" t="n">
-        <v>91.98985919471806</v>
+        <v>92.87074424098816</v>
       </c>
       <c r="C21" t="n">
-        <v>13.63684173648516</v>
+        <v>13.62732287984586</v>
       </c>
       <c r="D21" t="n">
-        <v>6.745686499286751</v>
+        <v>6.815039539302278</v>
       </c>
       <c r="E21" t="n">
-        <v>16.97686921275497</v>
+        <v>17.15141000856205</v>
       </c>
       <c r="F21" t="n">
-        <v>0.02578983631383612</v>
+        <v>0.02568245989232567</v>
       </c>
       <c r="G21" t="n">
-        <v>0.1662590820249301</v>
+        <v>0.2579465972585478</v>
       </c>
       <c r="H21" t="n">
         <v>23.84</v>
       </c>
       <c r="I21" t="n">
-        <v>0.6148296977218531</v>
+        <v>0.6122698438330439</v>
       </c>
       <c r="J21" t="n">
-        <v>23.22517030227815</v>
+        <v>23.22773015616696</v>
       </c>
       <c r="K21" t="n">
-        <v>4.095658957305103</v>
+        <v>4.096110376535733</v>
       </c>
       <c r="L21" t="n">
-        <v>27.32082925958325</v>
+        <v>27.32384053270269</v>
       </c>
       <c r="M21" t="n">
-        <v>6.731852329561312</v>
+        <v>6.732594307257943</v>
       </c>
       <c r="N21" t="n">
-        <v>20.58897693002194</v>
+        <v>20.59124622544475</v>
       </c>
       <c r="O21" t="n">
-        <v>2.63619337225621</v>
+        <v>2.636483930722211</v>
       </c>
       <c r="P21" t="n">
         <v>2.5167</v>
       </c>
       <c r="Q21" t="n">
-        <v>16.22438493367479</v>
+        <v>25.27694792641616</v>
       </c>
       <c r="R21" t="n">
-        <v>2.153822497938757</v>
+        <v>1.916752723627482</v>
       </c>
       <c r="S21" t="n">
-        <v>0.4720008950097438</v>
+        <v>0.4200480782099533</v>
       </c>
       <c r="T21" t="n">
-        <v>1.901701025080853</v>
+        <v>1.692382089442055</v>
       </c>
       <c r="U21" t="n">
-        <v>7.004032793266533</v>
+        <v>6.233103677632569</v>
       </c>
       <c r="V21" t="n">
-        <v>0.2334226974787406</v>
+        <v>0.2077300202672374</v>
       </c>
       <c r="W21" t="n">
-        <v>17.1523683573611</v>
+        <v>15.26441886325239</v>
       </c>
       <c r="X21" t="n">
-        <v>6.446690083710727</v>
+        <v>10.043687339141</v>
       </c>
       <c r="Y21" t="inlineStr">
         <is>

</xml_diff>